<commit_message>
Update Financial Performance Data.xlsx with new source data
</commit_message>
<xml_diff>
--- a/public/Financial Performance Data.xlsx
+++ b/public/Financial Performance Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kotzbauer/expense_management_analytics-RMT-v2/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{86E49570-BC3E-DC42-B3CF-67FFB361BFE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E505052-7799-2C4C-9905-B9DDE2C60D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6300" yWindow="7320" windowWidth="22840" windowHeight="10940" xr2:uid="{D14BF5B3-A1B2-8F41-B345-A936FB541A15}"/>
+    <workbookView xWindow="6220" yWindow="3300" windowWidth="22860" windowHeight="15400" xr2:uid="{D14BF5B3-A1B2-8F41-B345-A936FB541A15}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="116">
   <si>
     <t>Metric_ID</t>
   </si>
@@ -191,9 +191,6 @@
     <t>Calculated: (Total Revenue - Total Expenses) / Visit Count</t>
   </si>
   <si>
-    <t>CASHFLOW_AUG_VISIT_AVG</t>
-  </si>
-  <si>
     <t>August 2023/2024 Visit Average</t>
   </si>
   <si>
@@ -209,49 +206,184 @@
     <t>Dashboard Template Cashflow</t>
   </si>
   <si>
-    <t>CASHFLOW_AUG_VISIT_PROJ</t>
-  </si>
-  <si>
     <t>August 2025 Visit Projection</t>
   </si>
   <si>
     <t>Forecast</t>
   </si>
   <si>
-    <t>CASHFLOW_AUG_EXPENSES</t>
-  </si>
-  <si>
     <t>August 2025 Expected Expenses</t>
   </si>
   <si>
-    <t>CASHFLOW_AUG_REVENUE</t>
-  </si>
-  <si>
     <t>August 2025 Expected Revenue</t>
   </si>
   <si>
-    <t>CASHFLOW_AUG_PROFIT</t>
-  </si>
-  <si>
     <t>August 2025 Expected Profit</t>
   </si>
   <si>
-    <t>CASHFLOW_AUG_CASH_POSITION</t>
-  </si>
-  <si>
     <t>August 2025 End of Month Cash Position</t>
   </si>
   <si>
-    <t>CASHFLOW_DEC_VISIT_PROJ</t>
-  </si>
-  <si>
     <t>December 2025 Visit Projection</t>
   </si>
   <si>
-    <t>CASHFLOW_DEC_CASH_POSITION</t>
-  </si>
-  <si>
     <t>December 2025 End of Month Cash Position</t>
+  </si>
+  <si>
+    <t>CASHFLOW_AUGUST_VISIT_AVG</t>
+  </si>
+  <si>
+    <t>CASHFLOW_AUGUST_VISIT_PROJ</t>
+  </si>
+  <si>
+    <t>CASHFLOW_AUGUST_EXPENSES</t>
+  </si>
+  <si>
+    <t>CASHFLOW_AUGUST_REVENUE</t>
+  </si>
+  <si>
+    <t>CASHFLOW_AUGUST_PROFIT</t>
+  </si>
+  <si>
+    <t>CASHFLOW_AUGUST_CASH_POSITION</t>
+  </si>
+  <si>
+    <t>CASHFLOW_SEPTEMBER_VISIT_AVG</t>
+  </si>
+  <si>
+    <t>September 2023/2024 Visit Average</t>
+  </si>
+  <si>
+    <t>CASHFLOW_SEPTEMBER_VISIT_PROJ</t>
+  </si>
+  <si>
+    <t>September 2025 Visit Projection</t>
+  </si>
+  <si>
+    <t>CASHFLOW_SEPTEMBER_EXPENSES</t>
+  </si>
+  <si>
+    <t>September 2025 Expected Expenses</t>
+  </si>
+  <si>
+    <t>CASHFLOW_SEPTEMBER_REVENUE</t>
+  </si>
+  <si>
+    <t>September 2025 Expected Revenue</t>
+  </si>
+  <si>
+    <t>CASHFLOW_SEPTEMBER_PROFIT</t>
+  </si>
+  <si>
+    <t>September 2025 Expected Profit</t>
+  </si>
+  <si>
+    <t>CASHFLOW_SEPTEMBER_CASH_POSITION</t>
+  </si>
+  <si>
+    <t>September 2025 End of Month Cash Position</t>
+  </si>
+  <si>
+    <t>CASHFLOW_OCTOBER_VISIT_AVG</t>
+  </si>
+  <si>
+    <t>October 2023/2024 Visit Average</t>
+  </si>
+  <si>
+    <t>CASHFLOW_OCTOBER_VISIT_PROJ</t>
+  </si>
+  <si>
+    <t>October 2025 Visit Projection</t>
+  </si>
+  <si>
+    <t>CASHFLOW_OCTOBER_EXPENSES</t>
+  </si>
+  <si>
+    <t>October 2025 Expected Expenses</t>
+  </si>
+  <si>
+    <t>CASHFLOW_OCTOBER_REVENUE</t>
+  </si>
+  <si>
+    <t>October 2025 Expected Revenue</t>
+  </si>
+  <si>
+    <t>CASHFLOW_OCTOBER_PROFIT</t>
+  </si>
+  <si>
+    <t>October 2025 Expected Profit</t>
+  </si>
+  <si>
+    <t>CASHFLOW_OCTOBER_CASH_POSITION</t>
+  </si>
+  <si>
+    <t>October 2025 End of Month Cash Position</t>
+  </si>
+  <si>
+    <t>CASHFLOW_NOVEMBER_VISIT_AVG</t>
+  </si>
+  <si>
+    <t>November 2023/2024 Visit Average</t>
+  </si>
+  <si>
+    <t>CASHFLOW_NOVEMBER_VISIT_PROJ</t>
+  </si>
+  <si>
+    <t>November 2025 Visit Projection</t>
+  </si>
+  <si>
+    <t>CASHFLOW_NOVEMBER_EXPENSES</t>
+  </si>
+  <si>
+    <t>November 2025 Expected Expenses</t>
+  </si>
+  <si>
+    <t>CASHFLOW_NOVEMBER_REVENUE</t>
+  </si>
+  <si>
+    <t>November 2025 Expected Revenue</t>
+  </si>
+  <si>
+    <t>CASHFLOW_NOVEMBER_PROFIT</t>
+  </si>
+  <si>
+    <t>November 2025 Expected Profit</t>
+  </si>
+  <si>
+    <t>CASHFLOW_NOVEMBER_CASH_POSITION</t>
+  </si>
+  <si>
+    <t>November 2025 End of Month Cash Position</t>
+  </si>
+  <si>
+    <t>CASHFLOW_DECEMBER_VISIT_AVG</t>
+  </si>
+  <si>
+    <t>December 2023/2024 Visit Average</t>
+  </si>
+  <si>
+    <t>CASHFLOW_DECEMBER_VISIT_PROJ</t>
+  </si>
+  <si>
+    <t>CASHFLOW_DECEMBER_EXPENSES</t>
+  </si>
+  <si>
+    <t>December 2025 Expected Expenses</t>
+  </si>
+  <si>
+    <t>CASHFLOW_DECEMBER_REVENUE</t>
+  </si>
+  <si>
+    <t>December 2025 Expected Revenue</t>
+  </si>
+  <si>
+    <t>CASHFLOW_DECEMBER_PROFIT</t>
+  </si>
+  <si>
+    <t>December 2025 Expected Profit</t>
+  </si>
+  <si>
+    <t>CASHFLOW_DECEMBER_CASH_POSITION</t>
   </si>
 </sst>
 </file>
@@ -623,10 +755,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FBEFE19-61E6-F243-A9CA-2FBB70397F74}">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1028,234 +1160,872 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" t="s">
         <v>51</v>
       </c>
-      <c r="B13" t="s">
-        <v>52</v>
-      </c>
       <c r="C13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" t="s">
         <v>53</v>
-      </c>
-      <c r="D13" t="s">
-        <v>54</v>
       </c>
       <c r="E13">
         <v>840</v>
       </c>
       <c r="G13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I13" t="s">
         <v>22</v>
       </c>
       <c r="J13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F14">
         <v>1056</v>
       </c>
       <c r="G14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I14" t="s">
         <v>22</v>
       </c>
       <c r="J14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F15">
         <v>102064</v>
       </c>
       <c r="G15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I15" t="s">
         <v>14</v>
       </c>
       <c r="J15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B16" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F16">
         <v>120829</v>
       </c>
       <c r="G16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I16" t="s">
         <v>14</v>
       </c>
       <c r="J16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F17">
         <v>18765</v>
       </c>
       <c r="G17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I17" t="s">
         <v>14</v>
       </c>
       <c r="J17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B18" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F18">
         <v>293765</v>
       </c>
       <c r="G18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I18" t="s">
         <v>14</v>
       </c>
       <c r="J18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B19" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" t="s">
         <v>53</v>
       </c>
-      <c r="D19" t="s">
-        <v>59</v>
-      </c>
-      <c r="F19">
-        <v>1477</v>
+      <c r="E19">
+        <v>865</v>
       </c>
       <c r="G19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I19" t="s">
         <v>22</v>
       </c>
       <c r="J19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B20" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20">
+        <v>1087</v>
+      </c>
+      <c r="G20" t="s">
+        <v>54</v>
+      </c>
+      <c r="H20" t="s">
+        <v>54</v>
+      </c>
+      <c r="I20" t="s">
+        <v>22</v>
+      </c>
+      <c r="J20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21">
+        <v>105102</v>
+      </c>
+      <c r="G21" t="s">
+        <v>54</v>
+      </c>
+      <c r="H21" t="s">
+        <v>54</v>
+      </c>
+      <c r="I21" t="s">
+        <v>14</v>
+      </c>
+      <c r="J21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" t="s">
+        <v>57</v>
+      </c>
+      <c r="F22">
+        <v>124425</v>
+      </c>
+      <c r="G22" t="s">
+        <v>54</v>
+      </c>
+      <c r="H22" t="s">
+        <v>54</v>
+      </c>
+      <c r="I22" t="s">
+        <v>14</v>
+      </c>
+      <c r="J22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23">
+        <v>19324</v>
+      </c>
+      <c r="G23" t="s">
+        <v>54</v>
+      </c>
+      <c r="H23" t="s">
+        <v>54</v>
+      </c>
+      <c r="I23" t="s">
+        <v>14</v>
+      </c>
+      <c r="J23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>80</v>
+      </c>
+      <c r="B24" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" t="s">
+        <v>57</v>
+      </c>
+      <c r="F24">
+        <v>313089</v>
+      </c>
+      <c r="G24" t="s">
+        <v>54</v>
+      </c>
+      <c r="H24" t="s">
+        <v>54</v>
+      </c>
+      <c r="I24" t="s">
+        <v>14</v>
+      </c>
+      <c r="J24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" t="s">
         <v>53</v>
       </c>
-      <c r="D20" t="s">
-        <v>59</v>
-      </c>
-      <c r="F20">
+      <c r="E25">
+        <v>915</v>
+      </c>
+      <c r="G25" t="s">
+        <v>54</v>
+      </c>
+      <c r="H25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I25" t="s">
+        <v>22</v>
+      </c>
+      <c r="J25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>84</v>
+      </c>
+      <c r="B26" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" t="s">
+        <v>57</v>
+      </c>
+      <c r="F26">
+        <v>1150</v>
+      </c>
+      <c r="G26" t="s">
+        <v>54</v>
+      </c>
+      <c r="H26" t="s">
+        <v>54</v>
+      </c>
+      <c r="I26" t="s">
+        <v>22</v>
+      </c>
+      <c r="J26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>86</v>
+      </c>
+      <c r="B27" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" t="s">
+        <v>57</v>
+      </c>
+      <c r="F27">
+        <v>111177</v>
+      </c>
+      <c r="G27" t="s">
+        <v>54</v>
+      </c>
+      <c r="H27" t="s">
+        <v>54</v>
+      </c>
+      <c r="I27" t="s">
+        <v>14</v>
+      </c>
+      <c r="J27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>88</v>
+      </c>
+      <c r="B28" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" t="s">
+        <v>57</v>
+      </c>
+      <c r="F28">
+        <v>131618</v>
+      </c>
+      <c r="G28" t="s">
+        <v>54</v>
+      </c>
+      <c r="H28" t="s">
+        <v>54</v>
+      </c>
+      <c r="I28" t="s">
+        <v>14</v>
+      </c>
+      <c r="J28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>90</v>
+      </c>
+      <c r="B29" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" t="s">
+        <v>57</v>
+      </c>
+      <c r="F29">
+        <v>20441</v>
+      </c>
+      <c r="G29" t="s">
+        <v>54</v>
+      </c>
+      <c r="H29" t="s">
+        <v>54</v>
+      </c>
+      <c r="I29" t="s">
+        <v>14</v>
+      </c>
+      <c r="J29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>92</v>
+      </c>
+      <c r="B30" t="s">
+        <v>93</v>
+      </c>
+      <c r="C30" t="s">
+        <v>52</v>
+      </c>
+      <c r="D30" t="s">
+        <v>57</v>
+      </c>
+      <c r="F30">
+        <v>333530</v>
+      </c>
+      <c r="G30" t="s">
+        <v>54</v>
+      </c>
+      <c r="H30" t="s">
+        <v>54</v>
+      </c>
+      <c r="I30" t="s">
+        <v>14</v>
+      </c>
+      <c r="J30" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>94</v>
+      </c>
+      <c r="B31" t="s">
+        <v>95</v>
+      </c>
+      <c r="C31" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" t="s">
+        <v>53</v>
+      </c>
+      <c r="E31">
+        <v>950</v>
+      </c>
+      <c r="G31" t="s">
+        <v>54</v>
+      </c>
+      <c r="H31" t="s">
+        <v>54</v>
+      </c>
+      <c r="I31" t="s">
+        <v>22</v>
+      </c>
+      <c r="J31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>96</v>
+      </c>
+      <c r="B32" t="s">
+        <v>97</v>
+      </c>
+      <c r="C32" t="s">
+        <v>52</v>
+      </c>
+      <c r="D32" t="s">
+        <v>57</v>
+      </c>
+      <c r="F32">
+        <v>1194</v>
+      </c>
+      <c r="G32" t="s">
+        <v>54</v>
+      </c>
+      <c r="H32" t="s">
+        <v>54</v>
+      </c>
+      <c r="I32" t="s">
+        <v>22</v>
+      </c>
+      <c r="J32" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>98</v>
+      </c>
+      <c r="B33" t="s">
+        <v>99</v>
+      </c>
+      <c r="C33" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" t="s">
+        <v>57</v>
+      </c>
+      <c r="F33">
+        <v>115430</v>
+      </c>
+      <c r="G33" t="s">
+        <v>54</v>
+      </c>
+      <c r="H33" t="s">
+        <v>54</v>
+      </c>
+      <c r="I33" t="s">
+        <v>14</v>
+      </c>
+      <c r="J33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>100</v>
+      </c>
+      <c r="B34" t="s">
+        <v>101</v>
+      </c>
+      <c r="C34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D34" t="s">
+        <v>57</v>
+      </c>
+      <c r="F34">
+        <v>136652</v>
+      </c>
+      <c r="G34" t="s">
+        <v>54</v>
+      </c>
+      <c r="H34" t="s">
+        <v>54</v>
+      </c>
+      <c r="I34" t="s">
+        <v>14</v>
+      </c>
+      <c r="J34" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>102</v>
+      </c>
+      <c r="B35" t="s">
+        <v>103</v>
+      </c>
+      <c r="C35" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" t="s">
+        <v>57</v>
+      </c>
+      <c r="F35">
+        <v>21223</v>
+      </c>
+      <c r="G35" t="s">
+        <v>54</v>
+      </c>
+      <c r="H35" t="s">
+        <v>54</v>
+      </c>
+      <c r="I35" t="s">
+        <v>14</v>
+      </c>
+      <c r="J35" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>104</v>
+      </c>
+      <c r="B36" t="s">
+        <v>105</v>
+      </c>
+      <c r="C36" t="s">
+        <v>52</v>
+      </c>
+      <c r="D36" t="s">
+        <v>57</v>
+      </c>
+      <c r="F36">
+        <v>354752</v>
+      </c>
+      <c r="G36" t="s">
+        <v>54</v>
+      </c>
+      <c r="H36" t="s">
+        <v>54</v>
+      </c>
+      <c r="I36" t="s">
+        <v>14</v>
+      </c>
+      <c r="J36" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>106</v>
+      </c>
+      <c r="B37" t="s">
+        <v>107</v>
+      </c>
+      <c r="C37" t="s">
+        <v>52</v>
+      </c>
+      <c r="D37" t="s">
+        <v>53</v>
+      </c>
+      <c r="E37">
+        <v>1175</v>
+      </c>
+      <c r="G37" t="s">
+        <v>54</v>
+      </c>
+      <c r="H37" t="s">
+        <v>54</v>
+      </c>
+      <c r="I37" t="s">
+        <v>22</v>
+      </c>
+      <c r="J37" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>108</v>
+      </c>
+      <c r="B38" t="s">
+        <v>62</v>
+      </c>
+      <c r="C38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D38" t="s">
+        <v>57</v>
+      </c>
+      <c r="F38">
+        <v>1477</v>
+      </c>
+      <c r="G38" t="s">
+        <v>54</v>
+      </c>
+      <c r="H38" t="s">
+        <v>54</v>
+      </c>
+      <c r="I38" t="s">
+        <v>22</v>
+      </c>
+      <c r="J38" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>109</v>
+      </c>
+      <c r="B39" t="s">
+        <v>110</v>
+      </c>
+      <c r="C39" t="s">
+        <v>52</v>
+      </c>
+      <c r="D39" t="s">
+        <v>57</v>
+      </c>
+      <c r="F39">
+        <v>142768</v>
+      </c>
+      <c r="G39" t="s">
+        <v>54</v>
+      </c>
+      <c r="H39" t="s">
+        <v>54</v>
+      </c>
+      <c r="I39" t="s">
+        <v>14</v>
+      </c>
+      <c r="J39" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>111</v>
+      </c>
+      <c r="B40" t="s">
+        <v>112</v>
+      </c>
+      <c r="C40" t="s">
+        <v>52</v>
+      </c>
+      <c r="D40" t="s">
+        <v>57</v>
+      </c>
+      <c r="F40">
+        <v>169017</v>
+      </c>
+      <c r="G40" t="s">
+        <v>54</v>
+      </c>
+      <c r="H40" t="s">
+        <v>54</v>
+      </c>
+      <c r="I40" t="s">
+        <v>14</v>
+      </c>
+      <c r="J40" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>113</v>
+      </c>
+      <c r="B41" t="s">
+        <v>114</v>
+      </c>
+      <c r="C41" t="s">
+        <v>52</v>
+      </c>
+      <c r="D41" t="s">
+        <v>57</v>
+      </c>
+      <c r="F41">
+        <v>26249</v>
+      </c>
+      <c r="G41" t="s">
+        <v>54</v>
+      </c>
+      <c r="H41" t="s">
+        <v>54</v>
+      </c>
+      <c r="I41" t="s">
+        <v>14</v>
+      </c>
+      <c r="J41" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>115</v>
+      </c>
+      <c r="B42" t="s">
+        <v>63</v>
+      </c>
+      <c r="C42" t="s">
+        <v>52</v>
+      </c>
+      <c r="D42" t="s">
+        <v>57</v>
+      </c>
+      <c r="F42">
         <v>381001</v>
       </c>
-      <c r="G20" t="s">
-        <v>55</v>
-      </c>
-      <c r="H20" t="s">
-        <v>55</v>
-      </c>
-      <c r="I20" t="s">
-        <v>14</v>
-      </c>
-      <c r="J20" t="s">
-        <v>56</v>
+      <c r="G42" t="s">
+        <v>54</v>
+      </c>
+      <c r="H42" t="s">
+        <v>54</v>
+      </c>
+      <c r="I42" t="s">
+        <v>14</v>
+      </c>
+      <c r="J42" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore(data): update Financial Performance Data source file
</commit_message>
<xml_diff>
--- a/public/Financial Performance Data.xlsx
+++ b/public/Financial Performance Data.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kotzbauer/expense_management_analytics-Wilmington/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A9DF8917-361F-2B48-9C63-4ACC64CB3F0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7FC5CC5-B27A-C844-933F-0A992686E915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4380" yWindow="3300" windowWidth="22860" windowHeight="15400" xr2:uid="{D14BF5B3-A1B2-8F41-B345-A936FB541A15}"/>
+    <workbookView xWindow="4440" yWindow="3300" windowWidth="22860" windowHeight="15400" xr2:uid="{D14BF5B3-A1B2-8F41-B345-A936FB541A15}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -745,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FBEFE19-61E6-F243-A9CA-2FBB70397F74}">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H48"/>
+    <sheetView tabSelected="1" topLeftCell="B21" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13:F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -802,16 +802,16 @@
         <v>11</v>
       </c>
       <c r="E2">
-        <v>628429</v>
+        <v>729392</v>
       </c>
       <c r="F2">
-        <v>677245</v>
+        <v>779143</v>
       </c>
       <c r="G2">
-        <v>7.8E-2</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="H2">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -880,16 +880,16 @@
         <v>19</v>
       </c>
       <c r="E5">
-        <v>120903</v>
+        <v>198222</v>
       </c>
       <c r="F5">
-        <v>126810</v>
+        <v>192148</v>
       </c>
       <c r="G5">
-        <v>4.9000000000000002E-2</v>
+        <v>-3.1E-2</v>
       </c>
       <c r="H5">
-        <v>5</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -1068,10 +1068,10 @@
         <v>-1</v>
       </c>
       <c r="G12">
-        <v>-0.97499999999999998</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="H12">
-        <v>-98</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -1088,7 +1088,7 @@
         <v>38</v>
       </c>
       <c r="E13">
-        <v>798</v>
+        <v>566</v>
       </c>
       <c r="G13" t="s">
         <v>39</v>
@@ -1272,7 +1272,7 @@
         <v>41</v>
       </c>
       <c r="F21">
-        <v>63342</v>
+        <v>122566</v>
       </c>
       <c r="G21" t="s">
         <v>39</v>
@@ -1318,7 +1318,8 @@
         <v>41</v>
       </c>
       <c r="F23">
-        <v>-459</v>
+        <f>F22-F21</f>
+        <v>-59683</v>
       </c>
       <c r="G23" t="s">
         <v>39</v>
@@ -1341,7 +1342,7 @@
         <v>41</v>
       </c>
       <c r="F24">
-        <v>-1257</v>
+        <v>-18443</v>
       </c>
       <c r="G24" t="s">
         <v>39</v>
@@ -1410,7 +1411,7 @@
         <v>41</v>
       </c>
       <c r="F27">
-        <v>126270</v>
+        <v>126280</v>
       </c>
       <c r="G27" t="s">
         <v>39</v>
@@ -1479,7 +1480,7 @@
         <v>41</v>
       </c>
       <c r="F30">
-        <v>-2172</v>
+        <v>-19358</v>
       </c>
       <c r="G30" t="s">
         <v>39</v>
@@ -1548,7 +1549,7 @@
         <v>41</v>
       </c>
       <c r="F33">
-        <v>122544</v>
+        <v>122529</v>
       </c>
       <c r="G33" t="s">
         <v>39</v>
@@ -1571,7 +1572,7 @@
         <v>41</v>
       </c>
       <c r="F34">
-        <v>121656</v>
+        <v>121642</v>
       </c>
       <c r="G34" t="s">
         <v>39</v>
@@ -1617,7 +1618,7 @@
         <v>41</v>
       </c>
       <c r="F36">
-        <v>-3060</v>
+        <v>-20246</v>
       </c>
       <c r="G36" t="s">
         <v>39</v>
@@ -1686,7 +1687,7 @@
         <v>41</v>
       </c>
       <c r="F39">
-        <v>129720</v>
+        <v>129719</v>
       </c>
       <c r="G39" t="s">
         <v>39</v>
@@ -1709,7 +1710,7 @@
         <v>41</v>
       </c>
       <c r="F40">
-        <v>128780</v>
+        <v>128779</v>
       </c>
       <c r="G40" t="s">
         <v>39</v>
@@ -1755,7 +1756,7 @@
         <v>41</v>
       </c>
       <c r="F42">
-        <v>-4000</v>
+        <v>-21186</v>
       </c>
       <c r="G42" t="s">
         <v>39</v>
@@ -1893,7 +1894,7 @@
         <v>41</v>
       </c>
       <c r="F48">
-        <v>-4854</v>
+        <v>-22040</v>
       </c>
       <c r="G48" t="s">
         <v>39</v>

</xml_diff>